<commit_message>
15-03-205 update filds stepper and design
</commit_message>
<xml_diff>
--- a/excel-files/For CodeQuality.xlsx
+++ b/excel-files/For CodeQuality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/137050b3a10032a5/Desktop/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\live-projects\Credilly\excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB42BCA-9961-45AD-895C-A538ED7B8282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F3FCE1-DA98-4812-AC3B-8AE9BEB59194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{76E9DA6F-C589-421C-B0C3-7374B0280AAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{76E9DA6F-C589-421C-B0C3-7374B0280AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2158,6 +2158,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2212,50 +2257,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2263,54 +2311,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2320,12 +2326,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2334,6 +2334,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4923,8 +4929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725B0FE4-B528-43B3-8CA2-F72CC4265337}">
   <dimension ref="A2:S46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I29"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4944,13 +4950,13 @@
   <sheetData>
     <row r="2" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="5:17" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="72"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="87"/>
       <c r="J3" s="1" t="s">
         <v>460</v>
       </c>
@@ -4959,76 +4965,76 @@
       </c>
     </row>
     <row r="4" spans="5:17" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="73"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="75"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="90"/>
       <c r="L5" s="1" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="6" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="76"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="78"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="93"/>
       <c r="L6" s="1" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="7" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E7" s="79"/>
-      <c r="F7" s="79" t="s">
+      <c r="E7" s="94"/>
+      <c r="F7" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
     </row>
     <row r="8" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E8" s="80"/>
-      <c r="F8" s="80" t="s">
+      <c r="E8" s="95"/>
+      <c r="F8" s="95" t="s">
         <v>420</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
     </row>
     <row r="9" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E9" s="80"/>
-      <c r="F9" s="80" t="s">
+      <c r="E9" s="95"/>
+      <c r="F9" s="95" t="s">
         <v>421</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.3">
-      <c r="E10" s="80"/>
-      <c r="F10" s="80" t="s">
+      <c r="E10" s="95"/>
+      <c r="F10" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="86"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
     </row>
     <row r="11" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E11" s="81"/>
-      <c r="F11" s="81" t="s">
+      <c r="E11" s="96"/>
+      <c r="F11" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="87"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
     </row>
     <row r="12" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" s="4"/>
@@ -5047,7 +5053,7 @@
       </c>
     </row>
     <row r="13" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="93"/>
+      <c r="E13" s="75"/>
       <c r="F13" s="7" t="s">
         <v>4</v>
       </c>
@@ -5057,7 +5063,7 @@
       <c r="H13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="93"/>
+      <c r="I13" s="75"/>
       <c r="K13" s="1">
         <v>2</v>
       </c>
@@ -5082,11 +5088,11 @@
       </c>
     </row>
     <row r="14" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E14" s="94"/>
+      <c r="E14" s="76"/>
       <c r="F14" s="11"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="94"/>
+      <c r="I14" s="76"/>
       <c r="O14" s="1" t="s">
         <v>428</v>
       </c>
@@ -5098,14 +5104,14 @@
       </c>
     </row>
     <row r="15" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E15" s="94"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="94"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="5:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="94"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="15" t="s">
         <v>7</v>
       </c>
@@ -5115,7 +5121,7 @@
       <c r="H16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="94"/>
+      <c r="I16" s="76"/>
       <c r="K16" s="1" t="s">
         <v>431</v>
       </c>
@@ -5124,17 +5130,17 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E17" s="94"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="94"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="76"/>
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="94"/>
+      <c r="E18" s="76"/>
       <c r="F18" s="7" t="s">
         <v>11</v>
       </c>
@@ -5144,7 +5150,7 @@
       <c r="H18" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="94"/>
+      <c r="I18" s="76"/>
       <c r="K18" s="1" t="s">
         <v>433</v>
       </c>
@@ -5165,7 +5171,7 @@
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="94"/>
+      <c r="E19" s="76"/>
       <c r="F19" s="11" t="s">
         <v>15</v>
       </c>
@@ -5175,7 +5181,7 @@
       <c r="H19" s="13">
         <v>90000</v>
       </c>
-      <c r="I19" s="94"/>
+      <c r="I19" s="76"/>
       <c r="K19" s="1" t="s">
         <v>434</v>
       </c>
@@ -5190,11 +5196,11 @@
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="94"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="94"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="76"/>
       <c r="K20" s="1" t="s">
         <v>143</v>
       </c>
@@ -5209,7 +5215,7 @@
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="94"/>
+      <c r="E21" s="76"/>
       <c r="F21" s="15" t="s">
         <v>19</v>
       </c>
@@ -5219,23 +5225,23 @@
       <c r="H21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="94"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="94"/>
+      <c r="E22" s="76"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="94"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="94"/>
-      <c r="F23" s="99" t="s">
+      <c r="E23" s="76"/>
+      <c r="F23" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="94"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="76"/>
       <c r="K23" s="1" t="s">
         <v>23</v>
       </c>
@@ -5253,22 +5259,22 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="94"/>
-      <c r="F24" s="96" t="s">
+      <c r="E24" s="76"/>
+      <c r="F24" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="97"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="94"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="94"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="13"/>
       <c r="G25" s="14" t="s">
         <v>435</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="94"/>
+      <c r="I25" s="76"/>
       <c r="L25" s="1" t="s">
         <v>436</v>
       </c>
@@ -5280,44 +5286,44 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="94"/>
-      <c r="F26" s="100" t="s">
+      <c r="E26" s="76"/>
+      <c r="F26" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="101"/>
-      <c r="H26" s="102"/>
-      <c r="I26" s="94"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="76"/>
     </row>
     <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="94"/>
+      <c r="E27" s="76"/>
       <c r="F27" s="13"/>
       <c r="G27" s="14"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="94"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="94"/>
-      <c r="F28" s="96" t="s">
+      <c r="E28" s="76"/>
+      <c r="F28" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="97"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="94"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="95"/>
+      <c r="E29" s="77"/>
       <c r="F29" s="3"/>
       <c r="G29" s="21" t="s">
         <v>33</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="95"/>
+      <c r="I29" s="77"/>
       <c r="K29" s="1" t="s">
         <v>34</v>
       </c>
@@ -5329,28 +5335,28 @@
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="88" t="s">
+      <c r="E30" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="90"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
     </row>
     <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="129" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="129" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="129" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5358,19 +5364,19 @@
       <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="129" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="I32" s="129" t="s">
         <v>48</v>
       </c>
       <c r="K32" s="23" t="s">
@@ -5387,19 +5393,19 @@
       <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G33" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H33" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="130" t="s">
         <v>57</v>
       </c>
       <c r="O33" s="1" t="s">
@@ -5407,19 +5413,19 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="I34" s="129" t="s">
         <v>63</v>
       </c>
       <c r="O34" s="1" t="s">
@@ -5427,13 +5433,13 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E35" s="88" t="s">
+      <c r="E35" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="90"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
       <c r="O35" s="1" t="s">
         <v>16</v>
       </c>
@@ -5630,11 +5636,11 @@
       <c r="E46" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="F46" s="91" t="s">
+      <c r="F46" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="G46" s="92"/>
-      <c r="H46" s="92"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
       <c r="I46" s="20" t="s">
         <v>106</v>
       </c>
@@ -5653,6 +5659,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E3:I6"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="E30:I30"/>
     <mergeCell ref="E35:I35"/>
     <mergeCell ref="F46:H46"/>
@@ -5665,14 +5679,6 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F28:H28"/>
-    <mergeCell ref="E3:I6"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5683,8 +5689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020BD5E7-4FA5-4384-B702-7931298C46F5}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F51"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5887,7 +5893,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="105"/>
+      <c r="A12" s="116"/>
       <c r="B12" s="38" t="s">
         <v>143</v>
       </c>
@@ -5908,93 +5914,93 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="106"/>
-      <c r="B13" s="103" t="s">
+      <c r="A13" s="117"/>
+      <c r="B13" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="107">
+      <c r="D13" s="122">
         <v>4.65E-2</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="119" t="s">
         <v>150</v>
       </c>
-      <c r="F13" s="103" t="s">
+      <c r="F13" s="119" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="106"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
+      <c r="A14" s="117"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="106"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="111" t="s">
+      <c r="C16" s="110"/>
+      <c r="D16" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="113"/>
+      <c r="E16" s="111"/>
       <c r="F16" s="38" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="109"/>
-      <c r="B17" s="114" t="s">
+      <c r="A17" s="107"/>
+      <c r="B17" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="114" t="s">
+      <c r="C17" s="113"/>
+      <c r="D17" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="115"/>
+      <c r="E17" s="113"/>
       <c r="F17" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="110"/>
-      <c r="B18" s="116" t="s">
+      <c r="A18" s="108"/>
+      <c r="B18" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="116" t="s">
+      <c r="C18" s="115"/>
+      <c r="D18" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="117"/>
+      <c r="E18" s="115"/>
       <c r="F18" s="44" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="118"/>
-      <c r="B19" s="119"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="120"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="105"/>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="105"/>
+      <c r="A20" s="116"/>
       <c r="B20" s="29" t="s">
         <v>143</v>
       </c>
@@ -6012,93 +6018,93 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="106"/>
-      <c r="B21" s="103" t="s">
+      <c r="A21" s="117"/>
+      <c r="B21" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="103" t="s">
+      <c r="C21" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="107">
+      <c r="D21" s="122">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="E21" s="103" t="s">
+      <c r="E21" s="119" t="s">
         <v>162</v>
       </c>
-      <c r="F21" s="103" t="s">
+      <c r="F21" s="119" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="106"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="106"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="108" t="s">
+      <c r="A24" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="111" t="s">
+      <c r="B24" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="111" t="s">
+      <c r="C24" s="110"/>
+      <c r="D24" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="113"/>
+      <c r="E24" s="111"/>
       <c r="F24" s="38" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="109"/>
-      <c r="B25" s="114" t="s">
+      <c r="A25" s="107"/>
+      <c r="B25" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="115"/>
-      <c r="D25" s="114" t="s">
+      <c r="C25" s="113"/>
+      <c r="D25" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="115"/>
+      <c r="E25" s="113"/>
       <c r="F25" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="110"/>
-      <c r="B26" s="116" t="s">
+      <c r="A26" s="108"/>
+      <c r="B26" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="116" t="s">
+      <c r="C26" s="115"/>
+      <c r="D26" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="E26" s="117"/>
+      <c r="E26" s="115"/>
       <c r="F26" s="44" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="121"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="123"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="125"/>
     </row>
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="105"/>
+      <c r="A28" s="116"/>
       <c r="B28" s="29" t="s">
         <v>143</v>
       </c>
@@ -6116,93 +6122,93 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="106"/>
-      <c r="B29" s="103" t="s">
+      <c r="A29" s="117"/>
+      <c r="B29" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="D29" s="107">
+      <c r="D29" s="122">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E29" s="103" t="s">
+      <c r="E29" s="119" t="s">
         <v>164</v>
       </c>
-      <c r="F29" s="103" t="s">
+      <c r="F29" s="119" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="106"/>
-      <c r="B30" s="104"/>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="124"/>
-      <c r="B31" s="125"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
+      <c r="A31" s="118"/>
+      <c r="B31" s="121"/>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="108" t="s">
+      <c r="A32" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="111" t="s">
+      <c r="B32" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="112"/>
-      <c r="D32" s="111" t="s">
+      <c r="C32" s="110"/>
+      <c r="D32" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="113"/>
+      <c r="E32" s="111"/>
       <c r="F32" s="38" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="109"/>
-      <c r="B33" s="114" t="s">
+      <c r="A33" s="107"/>
+      <c r="B33" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="115"/>
-      <c r="D33" s="114" t="s">
+      <c r="C33" s="113"/>
+      <c r="D33" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E33" s="115"/>
+      <c r="E33" s="113"/>
       <c r="F33" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="110"/>
-      <c r="B34" s="116" t="s">
+      <c r="A34" s="108"/>
+      <c r="B34" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="116" t="s">
+      <c r="C34" s="115"/>
+      <c r="D34" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="E34" s="117"/>
+      <c r="E34" s="115"/>
       <c r="F34" s="44" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="118"/>
-      <c r="B35" s="119"/>
-      <c r="C35" s="119"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="120"/>
+      <c r="A35" s="103"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="105"/>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="105"/>
+      <c r="A36" s="116"/>
       <c r="B36" s="29" t="s">
         <v>143</v>
       </c>
@@ -6220,93 +6226,93 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="106"/>
-      <c r="B37" s="103" t="s">
+      <c r="A37" s="117"/>
+      <c r="B37" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="103" t="s">
+      <c r="C37" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="107">
+      <c r="D37" s="122">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="E37" s="103" t="s">
+      <c r="E37" s="119" t="s">
         <v>165</v>
       </c>
-      <c r="F37" s="103" t="s">
+      <c r="F37" s="119" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="106"/>
-      <c r="B38" s="104"/>
-      <c r="C38" s="104"/>
-      <c r="D38" s="104"/>
-      <c r="E38" s="104"/>
-      <c r="F38" s="104"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="120"/>
     </row>
     <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="124"/>
-      <c r="B39" s="125"/>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="125"/>
-      <c r="F39" s="125"/>
+      <c r="A39" s="118"/>
+      <c r="B39" s="121"/>
+      <c r="C39" s="121"/>
+      <c r="D39" s="121"/>
+      <c r="E39" s="121"/>
+      <c r="F39" s="121"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="108" t="s">
+      <c r="A40" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="B40" s="111" t="s">
+      <c r="B40" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="112"/>
-      <c r="D40" s="111" t="s">
+      <c r="C40" s="110"/>
+      <c r="D40" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="E40" s="113"/>
+      <c r="E40" s="111"/>
       <c r="F40" s="38" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="109"/>
-      <c r="B41" s="114" t="s">
+      <c r="A41" s="107"/>
+      <c r="B41" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C41" s="115"/>
-      <c r="D41" s="114" t="s">
+      <c r="C41" s="113"/>
+      <c r="D41" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E41" s="115"/>
+      <c r="E41" s="113"/>
       <c r="F41" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="110"/>
-      <c r="B42" s="116" t="s">
+      <c r="A42" s="108"/>
+      <c r="B42" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C42" s="117"/>
-      <c r="D42" s="116" t="s">
+      <c r="C42" s="115"/>
+      <c r="D42" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="E42" s="117"/>
+      <c r="E42" s="115"/>
       <c r="F42" s="44" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="118"/>
-      <c r="B43" s="119"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="120"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="105"/>
+      <c r="A44" s="116"/>
       <c r="B44" s="29" t="s">
         <v>143</v>
       </c>
@@ -6324,93 +6330,155 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="106"/>
-      <c r="B45" s="103" t="s">
+      <c r="A45" s="117"/>
+      <c r="B45" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="103" t="s">
+      <c r="C45" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="107">
+      <c r="D45" s="122">
         <v>5.5E-2</v>
       </c>
-      <c r="E45" s="103">
+      <c r="E45" s="119">
         <v>1630</v>
       </c>
-      <c r="F45" s="103" t="s">
+      <c r="F45" s="119" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="106"/>
-      <c r="B46" s="104"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="104"/>
-      <c r="F46" s="104"/>
+      <c r="A46" s="117"/>
+      <c r="B46" s="120"/>
+      <c r="C46" s="120"/>
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="120"/>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="124"/>
-      <c r="B47" s="125"/>
-      <c r="C47" s="125"/>
-      <c r="D47" s="125"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
+      <c r="A47" s="118"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="108" t="s">
+      <c r="A48" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="111" t="s">
+      <c r="C48" s="110"/>
+      <c r="D48" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="E48" s="113"/>
+      <c r="E48" s="111"/>
       <c r="F48" s="38" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="109"/>
-      <c r="B49" s="114" t="s">
+      <c r="A49" s="107"/>
+      <c r="B49" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="115"/>
-      <c r="D49" s="114" t="s">
+      <c r="C49" s="113"/>
+      <c r="D49" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E49" s="115"/>
+      <c r="E49" s="113"/>
       <c r="F49" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="110"/>
-      <c r="B50" s="116" t="s">
+      <c r="A50" s="108"/>
+      <c r="B50" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="117"/>
-      <c r="D50" s="116" t="s">
+      <c r="C50" s="115"/>
+      <c r="D50" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="E50" s="117"/>
+      <c r="E50" s="115"/>
       <c r="F50" s="44" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="118"/>
-      <c r="B51" s="119"/>
-      <c r="C51" s="119"/>
-      <c r="D51" s="119"/>
-      <c r="E51" s="119"/>
-      <c r="F51" s="120"/>
+      <c r="A51" s="103"/>
+      <c r="B51" s="104"/>
+      <c r="C51" s="104"/>
+      <c r="D51" s="104"/>
+      <c r="E51" s="104"/>
+      <c r="F51" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="F45:F47"/>
     <mergeCell ref="A51:F51"/>
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="B48:C48"/>
@@ -6419,68 +6487,6 @@
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6491,8 +6497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08171B03-F710-4D40-BDEA-59674D093DDA}">
   <dimension ref="B2:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6766,7 +6772,7 @@
       <c r="C21" s="126" t="s">
         <v>175</v>
       </c>
-      <c r="E21" s="105"/>
+      <c r="E21" s="116"/>
       <c r="F21" s="38" t="s">
         <v>143</v>
       </c>
@@ -6787,20 +6793,20 @@
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="48"/>
       <c r="C22" s="127"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="103" t="s">
+      <c r="E22" s="117"/>
+      <c r="F22" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="G22" s="103" t="s">
+      <c r="G22" s="119" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="107">
+      <c r="H22" s="122">
         <v>4.65E-2</v>
       </c>
-      <c r="I22" s="103" t="s">
+      <c r="I22" s="119" t="s">
         <v>150</v>
       </c>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="119" t="s">
         <v>151</v>
       </c>
       <c r="L22" s="51"/>
@@ -6808,70 +6814,70 @@
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="48"/>
       <c r="C23" s="127"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="104"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="104"/>
-      <c r="J23" s="104"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="120"/>
+      <c r="I23" s="120"/>
+      <c r="J23" s="120"/>
       <c r="L23" s="51"/>
     </row>
     <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="48"/>
       <c r="C24" s="127"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="125"/>
-      <c r="G24" s="125"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="125"/>
-      <c r="J24" s="125"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="121"/>
       <c r="L24" s="51"/>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="48"/>
       <c r="C25" s="127"/>
-      <c r="E25" s="108" t="s">
+      <c r="E25" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="F25" s="111" t="s">
+      <c r="F25" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="G25" s="112"/>
+      <c r="G25" s="110"/>
       <c r="H25" s="50"/>
-      <c r="I25" s="111" t="s">
+      <c r="I25" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="J25" s="112"/>
+      <c r="J25" s="110"/>
       <c r="L25" s="51"/>
     </row>
     <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="48"/>
       <c r="C26" s="127"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="114" t="s">
+      <c r="E26" s="107"/>
+      <c r="F26" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="G26" s="115"/>
+      <c r="G26" s="113"/>
       <c r="H26" s="52"/>
-      <c r="I26" s="114" t="s">
+      <c r="I26" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="J26" s="115"/>
+      <c r="J26" s="113"/>
       <c r="L26" s="51"/>
     </row>
     <row r="27" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="48"/>
       <c r="C27" s="128"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="116" t="s">
+      <c r="E27" s="108"/>
+      <c r="F27" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="G27" s="117"/>
+      <c r="G27" s="115"/>
       <c r="H27" s="54"/>
-      <c r="I27" s="116" t="s">
+      <c r="I27" s="114" t="s">
         <v>160</v>
       </c>
-      <c r="J27" s="117"/>
+      <c r="J27" s="115"/>
       <c r="L27" s="51"/>
     </row>
     <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7002,6 +7008,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="F22:F24"/>
     <mergeCell ref="H22:H24"/>
     <mergeCell ref="I22:I24"/>
     <mergeCell ref="J22:J24"/>
@@ -7013,11 +7024,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="G22:G24"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="F22:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>